<commit_message>
Importação da nova tabela de acústica
</commit_message>
<xml_diff>
--- a/data/EXCEL_acustica/acustica_PBC.xlsx
+++ b/data/EXCEL_acustica/acustica_PBC.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Saidas" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="356">
   <si>
     <t>BT- Begin Time</t>
   </si>
@@ -1284,6 +1284,9 @@
   <si>
     <t>0m40s</t>
   </si>
+  <si>
+    <t>"</t>
+  </si>
 </sst>
 </file>
 
@@ -35644,9 +35647,9 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P15"/>
+  <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
@@ -36269,6 +36272,11 @@
       </c>
       <c r="P15" s="49"/>
     </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="N16" s="91" t="s">
+        <v>355</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -36281,7 +36289,7 @@
   </sheetPr>
   <dimension ref="A1:X961"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="X9" sqref="X9"/>
     </sheetView>
   </sheetViews>

</xml_diff>